<commit_message>
Second Commit to Git Repository
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t>CHROME</t>
+  </si>
+  <si>
+    <t>16_05_2018_12_36_00</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>16_05_2018_12_38_01</t>
   </si>
 </sst>
 </file>
@@ -374,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,6 +423,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>

</xml_diff>